<commit_message>
added sound notification function, readme
</commit_message>
<xml_diff>
--- a/dnevnik.xlsx
+++ b/dnevnik.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Voronov\YandexDisk-euge.voronov@yandex.ru\Manual\Project\chasovoy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90461394-C3EE-45E4-9BB7-C70572EB8270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924AFD5-0884-4A05-B77E-132701DC05C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,78 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>29.06.2020</t>
+    <t>Дата</t>
   </si>
   <si>
-    <t>00:07:29</t>
-  </si>
-  <si>
-    <t>30.06.2020</t>
-  </si>
-  <si>
-    <t>01:34:46</t>
-  </si>
-  <si>
-    <t>01.07.2020</t>
-  </si>
-  <si>
-    <t>01:08:05</t>
-  </si>
-  <si>
-    <t>02.07.2020</t>
-  </si>
-  <si>
-    <t>01:36:55</t>
-  </si>
-  <si>
-    <t>03.07.2020</t>
-  </si>
-  <si>
-    <t>03:02:17</t>
-  </si>
-  <si>
-    <t>04.07.2020</t>
-  </si>
-  <si>
-    <t>02:55:42</t>
-  </si>
-  <si>
-    <t>05.07.2020</t>
-  </si>
-  <si>
-    <t>00:59:37</t>
-  </si>
-  <si>
-    <t>06.07.2020</t>
-  </si>
-  <si>
-    <t>00:41:44</t>
-  </si>
-  <si>
-    <t>07.07.2020</t>
-  </si>
-  <si>
-    <t>02:10:08</t>
-  </si>
-  <si>
-    <t>08.07.2020</t>
-  </si>
-  <si>
-    <t>01:27:35</t>
+    <t>Время</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -115,11 +70,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -397,98 +355,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B11"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>